<commit_message>
Update on 20250824 part 2
</commit_message>
<xml_diff>
--- a/直播源汇总文档/移动直播源/海南移动/海南移动.xlsx
+++ b/直播源汇总文档/移动直播源/海南移动/海南移动.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13825" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13867" uniqueCount="480">
   <si>
     <t>东方卫视</t>
   </si>
@@ -1493,6 +1493,14 @@
   </si>
   <si>
     <t>/000000001000/bokesen/</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电子竞技</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/200000001898/460000089800010084/</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -37310,7 +37318,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G439"/>
+  <dimension ref="A1:G445"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -47422,6 +47430,144 @@
         <v>428</v>
       </c>
     </row>
+    <row r="440" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A440" t="s">
+        <v>478</v>
+      </c>
+      <c r="B440" t="s">
+        <v>413</v>
+      </c>
+      <c r="C440" t="s">
+        <v>414</v>
+      </c>
+      <c r="D440" t="s">
+        <v>415</v>
+      </c>
+      <c r="E440" t="s">
+        <v>479</v>
+      </c>
+      <c r="F440" t="s">
+        <v>475</v>
+      </c>
+      <c r="G440" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="441" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A441" t="s">
+        <v>478</v>
+      </c>
+      <c r="B441" t="s">
+        <v>413</v>
+      </c>
+      <c r="C441" t="s">
+        <v>414</v>
+      </c>
+      <c r="D441" t="s">
+        <v>426</v>
+      </c>
+      <c r="E441" t="s">
+        <v>479</v>
+      </c>
+      <c r="F441" t="s">
+        <v>475</v>
+      </c>
+      <c r="G441" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="442" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A442" t="s">
+        <v>478</v>
+      </c>
+      <c r="B442" t="s">
+        <v>413</v>
+      </c>
+      <c r="C442" t="s">
+        <v>414</v>
+      </c>
+      <c r="D442" t="s">
+        <v>424</v>
+      </c>
+      <c r="E442" t="s">
+        <v>479</v>
+      </c>
+      <c r="F442" t="s">
+        <v>475</v>
+      </c>
+      <c r="G442" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="443" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A443" t="s">
+        <v>478</v>
+      </c>
+      <c r="B443" t="s">
+        <v>413</v>
+      </c>
+      <c r="C443" t="s">
+        <v>414</v>
+      </c>
+      <c r="D443" t="s">
+        <v>420</v>
+      </c>
+      <c r="E443" t="s">
+        <v>479</v>
+      </c>
+      <c r="F443" t="s">
+        <v>475</v>
+      </c>
+      <c r="G443" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="444" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A444" t="s">
+        <v>478</v>
+      </c>
+      <c r="B444" t="s">
+        <v>413</v>
+      </c>
+      <c r="C444" t="s">
+        <v>414</v>
+      </c>
+      <c r="D444" t="s">
+        <v>418</v>
+      </c>
+      <c r="E444" t="s">
+        <v>479</v>
+      </c>
+      <c r="F444" t="s">
+        <v>475</v>
+      </c>
+      <c r="G444" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="445" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A445" t="s">
+        <v>478</v>
+      </c>
+      <c r="B445" t="s">
+        <v>413</v>
+      </c>
+      <c r="C445" t="s">
+        <v>414</v>
+      </c>
+      <c r="D445" t="s">
+        <v>422</v>
+      </c>
+      <c r="E445" t="s">
+        <v>479</v>
+      </c>
+      <c r="F445" t="s">
+        <v>475</v>
+      </c>
+      <c r="G445" t="s">
+        <v>428</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:G439"/>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Update on 20250826 part 2
</commit_message>
<xml_diff>
--- a/直播源汇总文档/移动直播源/海南移动/海南移动.xlsx
+++ b/直播源汇总文档/移动直播源/海南移动/海南移动.xlsx
@@ -20,14 +20,14 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">体育!$A$1:$H$91</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">卫视!$A$1:$H$943</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">央视!$A$1:$H$607</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">娱乐!$A$1:$H$523</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">娱乐!$A$1:$H$529</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18834" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18882" uniqueCount="599">
   <si>
     <t>海南卫视</t>
   </si>
@@ -1855,6 +1855,18 @@
   <si>
     <t>NewTV热播精选</t>
   </si>
+  <si>
+    <t>ystenlive</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ystenlive</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bestzb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -1914,13 +1926,14 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -21371,7 +21384,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A129" s="1" t="s">
         <v>71</v>
       </c>
@@ -21394,7 +21407,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A130" s="1" t="s">
         <v>71</v>
       </c>
@@ -21417,7 +21430,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A131" s="1" t="s">
         <v>71</v>
       </c>
@@ -21440,7 +21453,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A132" s="1" t="s">
         <v>71</v>
       </c>
@@ -21463,7 +21476,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A133" s="1" t="s">
         <v>71</v>
       </c>
@@ -21486,7 +21499,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A134" s="1" t="s">
         <v>71</v>
       </c>
@@ -21509,7 +21522,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A135" s="1" t="s">
         <v>71</v>
       </c>
@@ -21532,7 +21545,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A136" s="1" t="s">
         <v>71</v>
       </c>
@@ -21555,7 +21568,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A137" s="1" t="s">
         <v>71</v>
       </c>
@@ -21578,7 +21591,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A138" s="1" t="s">
         <v>71</v>
       </c>
@@ -21601,7 +21614,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A139" s="1" t="s">
         <v>71</v>
       </c>
@@ -21624,7 +21637,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A140" s="1" t="s">
         <v>71</v>
       </c>
@@ -21646,8 +21659,11 @@
       <c r="G140" s="1" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H140" s="1" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A141" s="1" t="s">
         <v>71</v>
       </c>
@@ -21669,8 +21685,11 @@
       <c r="G141" s="1" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H141" s="1" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A142" s="1" t="s">
         <v>71</v>
       </c>
@@ -21692,8 +21711,11 @@
       <c r="G142" s="1" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H142" s="1" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A143" s="1" t="s">
         <v>71</v>
       </c>
@@ -21715,8 +21737,11 @@
       <c r="G143" s="1" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H143" s="1" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A144" s="1" t="s">
         <v>71</v>
       </c>
@@ -21738,8 +21763,11 @@
       <c r="G144" s="1" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H144" s="1" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A145" s="1" t="s">
         <v>71</v>
       </c>
@@ -21761,8 +21789,11 @@
       <c r="G145" s="1" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H145" s="1" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A146" s="1" t="s">
         <v>71</v>
       </c>
@@ -21784,8 +21815,11 @@
       <c r="G146" s="1" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H146" s="1" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A147" s="1" t="s">
         <v>71</v>
       </c>
@@ -21807,8 +21841,11 @@
       <c r="G147" s="1" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H147" s="1" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A148" s="1" t="s">
         <v>71</v>
       </c>
@@ -21830,8 +21867,11 @@
       <c r="G148" s="1" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H148" s="1" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A149" s="1" t="s">
         <v>71</v>
       </c>
@@ -21853,8 +21893,11 @@
       <c r="G149" s="1" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H149" s="1" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A150" s="1" t="s">
         <v>71</v>
       </c>
@@ -21876,8 +21919,11 @@
       <c r="G150" s="1" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H150" s="1" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A151" s="1" t="s">
         <v>71</v>
       </c>
@@ -21899,8 +21945,11 @@
       <c r="G151" s="1" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H151" s="1" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A152" s="1" t="s">
         <v>71</v>
       </c>
@@ -21922,8 +21971,11 @@
       <c r="G152" s="1" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H152" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A153" s="1" t="s">
         <v>71</v>
       </c>
@@ -21945,8 +21997,11 @@
       <c r="G153" s="1" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H153" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A154" s="1" t="s">
         <v>71</v>
       </c>
@@ -21968,8 +22023,11 @@
       <c r="G154" s="1" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H154" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A155" s="1" t="s">
         <v>71</v>
       </c>
@@ -21991,8 +22049,11 @@
       <c r="G155" s="1" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H155" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A156" s="1" t="s">
         <v>71</v>
       </c>
@@ -22014,8 +22075,11 @@
       <c r="G156" s="1" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H156" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A157" s="1" t="s">
         <v>71</v>
       </c>
@@ -22037,8 +22101,11 @@
       <c r="G157" s="1" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H157" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A158" s="1" t="s">
         <v>71</v>
       </c>
@@ -22060,8 +22127,11 @@
       <c r="G158" s="1" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H158" s="1" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A159" s="1" t="s">
         <v>71</v>
       </c>
@@ -22083,8 +22153,11 @@
       <c r="G159" s="1" t="s">
         <v>559</v>
       </c>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H159" s="1" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A160" s="1" t="s">
         <v>71</v>
       </c>
@@ -22105,6 +22178,9 @@
       </c>
       <c r="G160" s="1" t="s">
         <v>559</v>
+      </c>
+      <c r="H160" s="1" t="s">
+        <v>598</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.15">
@@ -22129,6 +22205,9 @@
       <c r="G161" s="1" t="s">
         <v>559</v>
       </c>
+      <c r="H161" s="1" t="s">
+        <v>598</v>
+      </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A162" s="1" t="s">
@@ -22152,6 +22231,9 @@
       <c r="G162" s="1" t="s">
         <v>559</v>
       </c>
+      <c r="H162" s="1" t="s">
+        <v>598</v>
+      </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A163" s="1" t="s">
@@ -22175,6 +22257,9 @@
       <c r="G163" s="1" t="s">
         <v>559</v>
       </c>
+      <c r="H163" s="1" t="s">
+        <v>598</v>
+      </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A164" s="1" t="s">
@@ -22198,6 +22283,9 @@
       <c r="G164" s="1" t="s">
         <v>564</v>
       </c>
+      <c r="H164" s="1" t="s">
+        <v>597</v>
+      </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A165" s="1" t="s">
@@ -22221,6 +22309,9 @@
       <c r="G165" s="1" t="s">
         <v>564</v>
       </c>
+      <c r="H165" s="1" t="s">
+        <v>597</v>
+      </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A166" s="1" t="s">
@@ -22244,6 +22335,9 @@
       <c r="G166" s="1" t="s">
         <v>564</v>
       </c>
+      <c r="H166" s="1" t="s">
+        <v>597</v>
+      </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A167" s="1" t="s">
@@ -22267,6 +22361,9 @@
       <c r="G167" s="1" t="s">
         <v>564</v>
       </c>
+      <c r="H167" s="1" t="s">
+        <v>597</v>
+      </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A168" s="1" t="s">
@@ -22290,6 +22387,9 @@
       <c r="G168" s="1" t="s">
         <v>564</v>
       </c>
+      <c r="H168" s="1" t="s">
+        <v>597</v>
+      </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A169" s="1" t="s">
@@ -22312,6 +22412,9 @@
       </c>
       <c r="G169" s="1" t="s">
         <v>564</v>
+      </c>
+      <c r="H169" s="1" t="s">
+        <v>597</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.15">
@@ -46599,6 +46702,9 @@
       <c r="G122" s="1" t="s">
         <v>554</v>
       </c>
+      <c r="H122" s="1" t="s">
+        <v>598</v>
+      </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A123" s="1" t="s">
@@ -46622,6 +46728,9 @@
       <c r="G123" s="1" t="s">
         <v>554</v>
       </c>
+      <c r="H123" s="1" t="s">
+        <v>598</v>
+      </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A124" s="1" t="s">
@@ -46645,6 +46754,9 @@
       <c r="G124" s="1" t="s">
         <v>554</v>
       </c>
+      <c r="H124" s="1" t="s">
+        <v>598</v>
+      </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A125" s="1" t="s">
@@ -46668,6 +46780,9 @@
       <c r="G125" s="1" t="s">
         <v>554</v>
       </c>
+      <c r="H125" s="1" t="s">
+        <v>598</v>
+      </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A126" s="1" t="s">
@@ -46691,6 +46806,9 @@
       <c r="G126" s="1" t="s">
         <v>554</v>
       </c>
+      <c r="H126" s="1" t="s">
+        <v>598</v>
+      </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A127" s="1" t="s">
@@ -46714,6 +46832,9 @@
       <c r="G127" s="1" t="s">
         <v>554</v>
       </c>
+      <c r="H127" s="1" t="s">
+        <v>598</v>
+      </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A128" s="1" t="s">
@@ -46737,6 +46858,9 @@
       <c r="G128" s="1" t="s">
         <v>554</v>
       </c>
+      <c r="H128" s="1" t="s">
+        <v>598</v>
+      </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A129" s="1" t="s">
@@ -46760,6 +46884,9 @@
       <c r="G129" s="1" t="s">
         <v>554</v>
       </c>
+      <c r="H129" s="1" t="s">
+        <v>598</v>
+      </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A130" s="1" t="s">
@@ -46783,6 +46910,9 @@
       <c r="G130" s="1" t="s">
         <v>554</v>
       </c>
+      <c r="H130" s="1" t="s">
+        <v>598</v>
+      </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A131" s="1" t="s">
@@ -46806,6 +46936,9 @@
       <c r="G131" s="1" t="s">
         <v>554</v>
       </c>
+      <c r="H131" s="1" t="s">
+        <v>598</v>
+      </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A132" s="1" t="s">
@@ -46829,6 +46962,9 @@
       <c r="G132" s="1" t="s">
         <v>554</v>
       </c>
+      <c r="H132" s="1" t="s">
+        <v>598</v>
+      </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A133" s="1" t="s">
@@ -46851,6 +46987,9 @@
       </c>
       <c r="G133" s="1" t="s">
         <v>554</v>
+      </c>
+      <c r="H133" s="1" t="s">
+        <v>598</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.15">
@@ -63183,6 +63322,9 @@
       <c r="G512" s="3" t="s">
         <v>532</v>
       </c>
+      <c r="H512" s="4" t="s">
+        <v>597</v>
+      </c>
     </row>
     <row r="513" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A513" s="3" t="s">
@@ -63206,6 +63348,9 @@
       <c r="G513" s="3" t="s">
         <v>532</v>
       </c>
+      <c r="H513" s="4" t="s">
+        <v>597</v>
+      </c>
     </row>
     <row r="514" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A514" s="3" t="s">
@@ -63229,6 +63374,9 @@
       <c r="G514" s="3" t="s">
         <v>532</v>
       </c>
+      <c r="H514" s="4" t="s">
+        <v>597</v>
+      </c>
     </row>
     <row r="515" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A515" s="3" t="s">
@@ -63252,6 +63400,9 @@
       <c r="G515" s="3" t="s">
         <v>532</v>
       </c>
+      <c r="H515" s="4" t="s">
+        <v>597</v>
+      </c>
     </row>
     <row r="516" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A516" s="3" t="s">
@@ -63275,6 +63426,9 @@
       <c r="G516" s="3" t="s">
         <v>532</v>
       </c>
+      <c r="H516" s="4" t="s">
+        <v>597</v>
+      </c>
     </row>
     <row r="517" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A517" s="3" t="s">
@@ -63298,6 +63452,9 @@
       <c r="G517" s="3" t="s">
         <v>532</v>
       </c>
+      <c r="H517" s="4" t="s">
+        <v>597</v>
+      </c>
     </row>
     <row r="518" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A518" t="s">
@@ -63594,7 +63751,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H505"/>
+  <autoFilter ref="A1:H529"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>